<commit_message>
remove original test cases
</commit_message>
<xml_diff>
--- a/Report/Report.xlsx
+++ b/Report/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>测试报告总概况</t>
   </si>
@@ -44,7 +44,7 @@
     <t>2017/12/4 13:00</t>
   </si>
   <si>
-    <t>2018-03-15 15:54:08</t>
+    <t>2018-03-22 17:17:09</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -59,7 +59,7 @@
     <t>测试耗时</t>
   </si>
   <si>
-    <t>113秒</t>
+    <t>193秒</t>
   </si>
   <si>
     <t>脚本语言</t>
@@ -119,21 +119,52 @@
     <t>testLogin</t>
   </si>
   <si>
-    <t>没有前置条件</t>
-  </si>
-  <si>
-    <t xml:space="preserve">确认手机权限
-输入用户名
+    <t>数据不清空，已登出</t>
+  </si>
+  <si>
+    <t xml:space="preserve">输入用户名
 输入密码
 点击登陆
 </t>
   </si>
   <si>
-    <t xml:space="preserve">检查更新日志弹框
+    <t xml:space="preserve">美容顾问姓名
 </t>
   </si>
   <si>
-    <t>testLogin2</t>
+    <t>浏览我的专属</t>
+  </si>
+  <si>
+    <t>testMyExclusive</t>
+  </si>
+  <si>
+    <t>已经登陆并停留在主页</t>
+  </si>
+  <si>
+    <t xml:space="preserve">打开我的订单
+取消设定促销时间
+打开我的专属
+打开全部订单
+打开成员订单状态
+返回上一级菜单
+打开全部订单
+返回上一级菜单
+打开最新订单
+返回上一级菜单
+返回主页
+</t>
+  </si>
+  <si>
+    <t>打开我的订单</t>
+  </si>
+  <si>
+    <t>testOpenOrderingUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">打开我的订单
+取消设定促销时间
+返回主页
+</t>
   </si>
 </sst>
 </file>
@@ -291,7 +322,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -689,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -706,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -759,7 +790,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -878,16 +909,16 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>36</v>
@@ -898,7 +929,34 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1"/>
+    <row r="5" spans="1:10" ht="30" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
     <row r="6" spans="1:10" ht="30" customHeight="1"/>
     <row r="7" spans="1:10" ht="30" customHeight="1"/>
     <row r="8" spans="1:10" ht="30" customHeight="1"/>

</xml_diff>